<commit_message>
working version; next step group data by player
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="4">
   <si>
     <t>takeoff</t>
   </si>
@@ -74,7 +74,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="79">
+  <borders count="99">
     <border>
       <left/>
       <right/>
@@ -160,11 +160,31 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -244,6 +264,26 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="85" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="86" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="87" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="88" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="89" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="90" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="91" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="92" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="93" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="94" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="95" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="96" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="97" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="98" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,25 +577,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="38">
-        <v>43955.426037384263</v>
-      </c>
-      <c r="B2" s="38">
-        <v>43955.426040856481</v>
+      <c r="A1" s="79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="80">
+        <v>43958.426037384263</v>
+      </c>
+      <c r="B2" s="80">
+        <v>43958.426040856481</v>
       </c>
       <c r="C2">
         <v>0.30000000000000071</v>
@@ -589,25 +629,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="55" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="56">
-        <v>43955.436869675927</v>
-      </c>
-      <c r="B2" s="56">
-        <v>43955.436872800929</v>
+      <c r="A1" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="97" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="97" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="97" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="98">
+        <v>43958.436869675927</v>
+      </c>
+      <c r="B2" s="98">
+        <v>43958.436872800929</v>
       </c>
       <c r="C2">
         <v>0.27000000000000046</v>
@@ -1041,30 +1081,30 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="40">
-        <v>43955.427804166669</v>
+      <c r="A1" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="82">
+        <v>43958.427804166669</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="40">
-        <v>43955.42801747685</v>
+      <c r="A3" s="82">
+        <v>43958.42801747685</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1172,25 +1212,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="42">
-        <v>43955.428610995368</v>
-      </c>
-      <c r="B2" s="42">
-        <v>43955.428612268515</v>
+      <c r="A1" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="83" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="84">
+        <v>43958.428610995368</v>
+      </c>
+      <c r="B2" s="84">
+        <v>43958.428612268515</v>
       </c>
       <c r="C2">
         <v>0.10999999999999943</v>
@@ -1215,22 +1255,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="43" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="44">
-        <v>43955.429490046299</v>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="85" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="86">
+        <v>43958.429490046299</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1252,30 +1292,30 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="46">
-        <v>43955.431137847219</v>
+      <c r="A1" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="88">
+        <v>43958.431137847219</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="46">
-        <v>43955.431248958332</v>
+      <c r="A3" s="88">
+        <v>43958.431248958332</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1297,25 +1337,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="48">
-        <v>43955.432224537035</v>
-      </c>
-      <c r="B2" s="48">
-        <v>43955.432234143518</v>
+      <c r="A1" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="89" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="90">
+        <v>43958.432224537035</v>
+      </c>
+      <c r="B2" s="90">
+        <v>43958.432234143518</v>
       </c>
       <c r="C2">
         <v>0.83000000000000185</v>
@@ -1340,25 +1380,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="50">
-        <v>43955.433753703706</v>
-      </c>
-      <c r="B2" s="50">
-        <v>43955.43376388889</v>
+      <c r="A1" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="91" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="91" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="92">
+        <v>43958.433753703706</v>
+      </c>
+      <c r="B2" s="92">
+        <v>43958.43376388889</v>
       </c>
       <c r="C2">
         <v>0.88000000000000256</v>
@@ -1383,25 +1423,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="52">
-        <v>43955.434179398151</v>
-      </c>
-      <c r="B2" s="52">
-        <v>43955.434185995371</v>
+      <c r="A1" s="93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="93" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="94">
+        <v>43958.434179398151</v>
+      </c>
+      <c r="B2" s="94">
+        <v>43958.434185995371</v>
       </c>
       <c r="C2">
         <v>0.57000000000000028</v>
@@ -1440,25 +1480,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="53" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="53" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="54">
-        <v>43955.435435300926</v>
-      </c>
-      <c r="B2" s="54">
-        <v>43955.43544548611</v>
+      <c r="A1" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="95" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="95" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="96">
+        <v>43958.435435300926</v>
+      </c>
+      <c r="B2" s="96">
+        <v>43958.43544548611</v>
       </c>
       <c r="C2">
         <v>0.88000000000000034</v>

</xml_diff>